<commit_message>
Running z_score MIR code with manual spurious epochs removal and not 2nd max & min
</commit_message>
<xml_diff>
--- a/AGN_outlier_flux.xlsx
+++ b/AGN_outlier_flux.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\Level-4-Project\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\New_project_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{C0D43A74-46D9-42C2-93B8-4AA17A572D70}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E6492E-483A-45CF-A229-8F13A53E5037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3982AA47-A081-4433-BC05-43D683ECED93}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="53" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
   <si>
     <t>AGN</t>
   </si>
@@ -123,9 +123,6 @@
   </si>
   <si>
     <t>Epoch</t>
-  </si>
-  <si>
-    <t>W3</t>
   </si>
 </sst>
 </file>
@@ -515,7 +512,7 @@
   <dimension ref="A1:C27"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="F18" sqref="F18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -579,6 +576,9 @@
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>6</v>
+      </c>
       <c r="B6" t="s">
         <v>2</v>
       </c>
@@ -642,8 +642,11 @@
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>11</v>
+      </c>
       <c r="B12" t="s">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="C12">
         <v>13</v>

</xml_diff>

<commit_message>
Fixed epoch removal code
</commit_message>
<xml_diff>
--- a/AGN_outlier_flux.xlsx
+++ b/AGN_outlier_flux.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ciara\Dropbox\University\University Work\Fourth Year\Project\New_project_repository\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E6492E-483A-45CF-A229-8F13A53E5037}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F13CA7FC-3E0B-4334-9B65-93731AC2A135}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{3982AA47-A081-4433-BC05-43D683ECED93}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="29">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="31">
   <si>
     <t>AGN</t>
   </si>
@@ -56,9 +56,6 @@
     <t>W1</t>
   </si>
   <si>
-    <t xml:space="preserve">111353.73+515725.8 </t>
-  </si>
-  <si>
     <t>112934.69+503103.4</t>
   </si>
   <si>
@@ -123,6 +120,15 @@
   </si>
   <si>
     <t>Epoch</t>
+  </si>
+  <si>
+    <t>141648.88+530903.5</t>
+  </si>
+  <si>
+    <t>111353.73+515725.8</t>
+  </si>
+  <si>
+    <t>125731.87+272313.3</t>
   </si>
 </sst>
 </file>
@@ -509,10 +515,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{26919F45-0A23-4466-9145-3DB570C207C3}">
-  <dimension ref="A1:C27"/>
+  <dimension ref="A1:C30"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F18" sqref="F18"/>
+    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -525,10 +531,10 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="C1" s="1" t="s">
         <v>27</v>
-      </c>
-      <c r="C1" s="1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
@@ -566,7 +572,7 @@
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B5" t="s">
         <v>5</v>
@@ -577,7 +583,7 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>29</v>
       </c>
       <c r="B6" t="s">
         <v>2</v>
@@ -588,7 +594,7 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>2</v>
@@ -599,7 +605,7 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>2</v>
@@ -610,7 +616,7 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>2</v>
@@ -621,7 +627,7 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>2</v>
@@ -632,7 +638,7 @@
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11" t="s">
         <v>2</v>
@@ -643,7 +649,7 @@
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>2</v>
@@ -654,7 +660,7 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>2</v>
@@ -665,7 +671,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>5</v>
@@ -676,117 +682,117 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="B15" t="s">
         <v>5</v>
       </c>
       <c r="C15">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C16">
-        <v>21</v>
+        <v>5</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B17" t="s">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="C17">
-        <v>14</v>
+        <v>21</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
       <c r="B18" t="s">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="C18">
-        <v>16</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
-        <v>18</v>
+        <v>16</v>
       </c>
       <c r="B19" t="s">
         <v>2</v>
       </c>
       <c r="C19">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="20" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B20" t="s">
         <v>2</v>
       </c>
       <c r="C20">
-        <v>10</v>
+        <v>23</v>
       </c>
     </row>
     <row r="21" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B21" t="s">
         <v>2</v>
       </c>
       <c r="C21">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="22" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B22" t="s">
         <v>2</v>
       </c>
       <c r="C22">
-        <v>10</v>
+        <v>25</v>
       </c>
     </row>
     <row r="23" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B23" t="s">
         <v>2</v>
       </c>
       <c r="C23">
-        <v>25</v>
+        <v>10</v>
       </c>
     </row>
     <row r="24" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B24" t="s">
         <v>2</v>
       </c>
       <c r="C24">
-        <v>13</v>
+        <v>25</v>
       </c>
     </row>
     <row r="25" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B25" t="s">
         <v>2</v>
@@ -797,24 +803,57 @@
     </row>
     <row r="26" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B26" t="s">
         <v>2</v>
       </c>
       <c r="C26">
-        <v>24</v>
+        <v>13</v>
       </c>
     </row>
     <row r="27" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B27" t="s">
         <v>2</v>
       </c>
       <c r="C27">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="28" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>25</v>
+      </c>
+      <c r="B28" t="s">
+        <v>2</v>
+      </c>
+      <c r="C28">
         <v>12</v>
+      </c>
+    </row>
+    <row r="29" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>28</v>
+      </c>
+      <c r="B29" t="s">
+        <v>5</v>
+      </c>
+      <c r="C29">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="30" spans="1:3" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>30</v>
+      </c>
+      <c r="B30" t="s">
+        <v>5</v>
+      </c>
+      <c r="C30">
+        <v>6</v>
       </c>
     </row>
   </sheetData>

</xml_diff>